<commit_message>
Second day of PacMan || Read Map From Archive and More Details on Draw
</commit_message>
<xml_diff>
--- a/PacManMap.xlsx
+++ b/PacManMap.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Office Desktop\Desktop\2022.1\Computação Gráfica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Office Desktop\github\pac-man-3D\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4FF715B-C320-4964-B056-D705A2908F14}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EDA2784-8902-40D1-861C-1E01013409D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{8235B0A7-1113-486B-8D2F-02D37F20FBA0}"/>
   </bookViews>
@@ -477,13 +477,13 @@
   <dimension ref="A1:X24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+      <selection sqref="A1:T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="21" width="5.7109375" style="2" customWidth="1"/>
-    <col min="22" max="24" width="5.7109375" style="2" hidden="1"/>
+    <col min="1" max="20" width="5.7109375" style="2" customWidth="1"/>
+    <col min="21" max="24" width="5.7109375" style="2" hidden="1" customWidth="1"/>
     <col min="25" max="16384" width="9.140625" style="2" hidden="1"/>
   </cols>
   <sheetData>
@@ -611,7 +611,7 @@
         <v>2</v>
       </c>
       <c r="T2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U2" s="1">
         <v>1</v>
@@ -670,13 +670,13 @@
         <v>1</v>
       </c>
       <c r="R3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U3" s="1">
         <v>1</v>
@@ -735,13 +735,13 @@
         <v>1</v>
       </c>
       <c r="R4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U4" s="1">
         <v>1</v>
@@ -800,13 +800,13 @@
         <v>2</v>
       </c>
       <c r="R5" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S5" s="1">
         <v>2</v>
       </c>
       <c r="T5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U5" s="1">
         <v>1</v>
@@ -859,13 +859,13 @@
         <v>1</v>
       </c>
       <c r="P6" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q6" s="1">
         <v>1</v>
       </c>
       <c r="R6" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S6" s="1">
         <v>1</v>
@@ -927,16 +927,16 @@
         <v>2</v>
       </c>
       <c r="Q7" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R7" s="1">
         <v>2</v>
       </c>
       <c r="S7" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T7" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U7" s="1">
         <v>1</v>
@@ -995,13 +995,13 @@
         <v>2</v>
       </c>
       <c r="R8" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S8" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T8" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U8" s="1">
         <v>1</v>
@@ -1057,16 +1057,16 @@
         <v>2</v>
       </c>
       <c r="Q9" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R9" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S9" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T9" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U9" s="1">
         <v>1</v>
@@ -1125,13 +1125,13 @@
         <v>1</v>
       </c>
       <c r="R10" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S10" s="1">
         <v>2</v>
       </c>
       <c r="T10" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U10" s="1">
         <v>1</v>
@@ -1243,7 +1243,7 @@
         <v>1</v>
       </c>
       <c r="N12" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O12" s="1">
         <v>1</v>
@@ -1261,7 +1261,7 @@
         <v>2</v>
       </c>
       <c r="T12" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U12" s="1">
         <v>1</v>
@@ -1323,10 +1323,10 @@
         <v>1</v>
       </c>
       <c r="S13" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T13" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U13" s="1">
         <v>1</v>
@@ -1382,7 +1382,7 @@
         <v>2</v>
       </c>
       <c r="Q14" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R14" s="1">
         <v>2</v>
@@ -1391,7 +1391,7 @@
         <v>2</v>
       </c>
       <c r="T14" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U14" s="1">
         <v>1</v>
@@ -1447,16 +1447,16 @@
         <v>2</v>
       </c>
       <c r="Q15" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R15" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S15" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T15" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U15" s="1">
         <v>1</v>
@@ -1515,13 +1515,13 @@
         <v>1</v>
       </c>
       <c r="R16" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S16" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T16" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U16" s="1">
         <v>1</v>
@@ -1583,10 +1583,10 @@
         <v>2</v>
       </c>
       <c r="S17" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T17" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U17" s="1">
         <v>1</v>
@@ -1639,7 +1639,7 @@
         <v>2</v>
       </c>
       <c r="P18" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q18" s="1">
         <v>1</v>
@@ -1648,10 +1648,10 @@
         <v>1</v>
       </c>
       <c r="S18" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T18" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U18" s="1">
         <v>1</v>
@@ -1716,7 +1716,7 @@
         <v>2</v>
       </c>
       <c r="T19" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="U19" s="1">
         <v>1</v>
@@ -1727,37 +1727,37 @@
         <v>1</v>
       </c>
       <c r="B20" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20" s="1">
         <v>1</v>
       </c>
       <c r="D20" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20" s="1">
         <v>1</v>
       </c>
       <c r="F20" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G20" s="1">
         <v>1</v>
       </c>
       <c r="H20" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I20" s="1">
         <v>1</v>
       </c>
       <c r="J20" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K20" s="1">
         <v>1</v>
       </c>
       <c r="L20" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M20" s="1">
         <v>1</v>
@@ -1781,142 +1781,14 @@
         <v>1</v>
       </c>
       <c r="T20" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U20" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>1</v>
-      </c>
-      <c r="B21" s="1">
-        <v>2</v>
-      </c>
-      <c r="C21" s="1">
-        <v>2</v>
-      </c>
-      <c r="D21" s="1">
-        <v>2</v>
-      </c>
-      <c r="E21" s="1">
-        <v>2</v>
-      </c>
-      <c r="F21" s="1">
-        <v>2</v>
-      </c>
-      <c r="G21" s="1">
-        <v>1</v>
-      </c>
-      <c r="H21" s="1">
-        <v>2</v>
-      </c>
-      <c r="I21" s="1">
-        <v>2</v>
-      </c>
-      <c r="J21" s="1">
-        <v>2</v>
-      </c>
-      <c r="K21" s="1">
-        <v>2</v>
-      </c>
-      <c r="L21" s="1">
-        <v>2</v>
-      </c>
-      <c r="M21" s="1">
-        <v>2</v>
-      </c>
-      <c r="N21" s="1">
-        <v>2</v>
-      </c>
-      <c r="O21" s="1">
-        <v>2</v>
-      </c>
-      <c r="P21" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q21" s="1">
-        <v>2</v>
-      </c>
-      <c r="R21" s="1">
-        <v>2</v>
-      </c>
-      <c r="S21" s="1">
-        <v>2</v>
-      </c>
-      <c r="T21" s="1">
-        <v>2</v>
-      </c>
-      <c r="U21" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>1</v>
-      </c>
-      <c r="B22" s="1">
-        <v>1</v>
-      </c>
-      <c r="C22" s="1">
-        <v>1</v>
-      </c>
-      <c r="D22" s="1">
-        <v>1</v>
-      </c>
-      <c r="E22" s="1">
-        <v>1</v>
-      </c>
-      <c r="F22" s="1">
-        <v>1</v>
-      </c>
-      <c r="G22" s="1">
-        <v>1</v>
-      </c>
-      <c r="H22" s="1">
-        <v>1</v>
-      </c>
-      <c r="I22" s="1">
-        <v>1</v>
-      </c>
-      <c r="J22" s="1">
-        <v>1</v>
-      </c>
-      <c r="K22" s="1">
-        <v>1</v>
-      </c>
-      <c r="L22" s="1">
-        <v>1</v>
-      </c>
-      <c r="M22" s="1">
-        <v>1</v>
-      </c>
-      <c r="N22" s="1">
-        <v>1</v>
-      </c>
-      <c r="O22" s="1">
-        <v>1</v>
-      </c>
-      <c r="P22" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q22" s="1">
-        <v>1</v>
-      </c>
-      <c r="R22" s="1">
-        <v>1</v>
-      </c>
-      <c r="S22" s="1">
-        <v>1</v>
-      </c>
-      <c r="T22" s="1">
-        <v>1</v>
-      </c>
-      <c r="U22" s="1">
-        <v>1</v>
-      </c>
-    </row>
+    <row r="21" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>

</xml_diff>

<commit_message>
Added Texture and Lighting to Game
</commit_message>
<xml_diff>
--- a/PacManMap.xlsx
+++ b/PacManMap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Office Desktop\github\pac-man-3D\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EDA2784-8902-40D1-861C-1E01013409D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B295EBA-43AB-4B1D-B567-B1AA10BA6CFE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{8235B0A7-1113-486B-8D2F-02D37F20FBA0}"/>
   </bookViews>
@@ -477,7 +477,7 @@
   <dimension ref="A1:X24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:T20"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -773,7 +773,7 @@
         <v>2</v>
       </c>
       <c r="I5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J5" s="1">
         <v>2</v>
@@ -832,7 +832,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H6" s="1">
         <v>2</v>
@@ -1665,19 +1665,19 @@
         <v>2</v>
       </c>
       <c r="C19" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D19" s="1">
         <v>2</v>
       </c>
       <c r="E19" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F19" s="1">
         <v>2</v>
       </c>
       <c r="G19" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H19" s="1">
         <v>2</v>
@@ -1689,7 +1689,7 @@
         <v>2</v>
       </c>
       <c r="K19" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L19" s="1">
         <v>2</v>

</xml_diff>

<commit_message>
Added Win Condition and Pacman Death
</commit_message>
<xml_diff>
--- a/PacManMap.xlsx
+++ b/PacManMap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Office Desktop\github\pac-man-3D\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B295EBA-43AB-4B1D-B567-B1AA10BA6CFE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192452C7-1DD9-41C9-B8BC-E0D358CD114E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{8235B0A7-1113-486B-8D2F-02D37F20FBA0}"/>
   </bookViews>
@@ -477,7 +477,7 @@
   <dimension ref="A1:X24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1036,13 +1036,13 @@
         <v>1</v>
       </c>
       <c r="J9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K9" s="1">
         <v>8</v>
       </c>
       <c r="L9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M9" s="1">
         <v>1</v>

</xml_diff>